<commit_message>
updating the varscan output for r1
</commit_message>
<xml_diff>
--- a/h5n1-hpai/STable-X_bald-eagle.xlsx
+++ b/h5n1-hpai/STable-X_bald-eagle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tavis.anderson/Desktop/local-repos/datasets/h5n1-hpai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FFF3CA-6870-AE44-938F-6B609C66CC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7F528C-6F20-C947-86D6-D752CF222712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40080" yWindow="1920" windowWidth="41560" windowHeight="25160" xr2:uid="{6588293A-AC02-B349-BA67-FE01579C41EC}"/>
   </bookViews>

</xml_diff>